<commit_message>
fix typo in creator id
</commit_message>
<xml_diff>
--- a/data/publisher_peer_review/xlsx/peer_review_elife.xlsx
+++ b/data/publisher_peer_review/xlsx/peer_review_elife.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t xml:space="preserve">creator</t>
   </si>
   <si>
-    <t xml:space="preserve">https://elifesciences.org/</t>
+    <t xml:space="preserve">https://elifesciences.org</t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t xml:space="preserve">2050-084X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://elifesciences.org</t>
   </si>
 </sst>
 </file>
@@ -426,8 +423,8 @@
   </sheetPr>
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA12" activeCellId="0" sqref="AA12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -438,7 +435,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="8.83"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -659,7 +656,7 @@
         <v>40</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>0</v>
@@ -724,7 +721,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F7" r:id="rId1" display="https://elifesciences.org"/>
+    <hyperlink ref="B1" r:id="rId1" display="https://elifesciences.org"/>
+    <hyperlink ref="F7" r:id="rId2" display="https://elifesciences.org"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>